<commit_message>
working on table formatin
</commit_message>
<xml_diff>
--- a/doc/Supplemental_Tables.xlsx
+++ b/doc/Supplemental_Tables.xlsx
@@ -28,7 +28,7 @@
     <definedName name="ABS.IFD_Q1_M1" localSheetId="9">'Q1 IFD'!$A$2:$E$3</definedName>
     <definedName name="ABS.IFD_Q1_M2" localSheetId="9">'Q1 IFD'!$A$6:$E$20</definedName>
     <definedName name="ABS.IFD_Q1_M3" localSheetId="9">'Q1 IFD'!$A$24:$E$39</definedName>
-    <definedName name="MLH1_M1_glm" localSheetId="1">'MLH1.M1_models'!$B$2:$E$3</definedName>
+    <definedName name="MLH1_M1_glm" localSheetId="1">'MLH1.M1_models'!#REF!</definedName>
     <definedName name="MLH1_M1_glm" localSheetId="0">MLH1_M1!$B$1:$E$2</definedName>
     <definedName name="MLH1_M2_glm" localSheetId="2">MLH1_M2!$A$1:$E$17</definedName>
     <definedName name="MLH1_M3_glm" localSheetId="3">MLH1_M3!#REF!</definedName>
@@ -103,8 +103,8 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="5" name="MLH1_M1_glm1" type="6" refreshedVersion="5" background="1" saveData="1">
-    <textPr codePage="437" sourceFile="C:\Users\April\Documents\MLH1repo\MLH1_M1_glm.csv" comma="1">
+  <connection id="5" name="MLH1_M2_glm" type="6" refreshedVersion="5" background="1" saveData="1">
+    <textPr codePage="437" sourceFile="C:\Users\April\Documents\MLH1repo\MLH1_M2_glm.csv" comma="1">
       <textFields count="5">
         <textField/>
         <textField/>
@@ -114,8 +114,8 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="6" name="MLH1_M2_glm" type="6" refreshedVersion="5" background="1" saveData="1">
-    <textPr codePage="437" sourceFile="C:\Users\April\Documents\MLH1repo\MLH1_M2_glm.csv" comma="1">
+  <connection id="6" name="MLH1_M4_female_glm" type="6" refreshedVersion="5" background="1" saveData="1">
+    <textPr codePage="437" sourceFile="C:\Users\April\Documents\MLH1repo\MLH1_M4_female_glm.csv" comma="1">
       <textFields count="5">
         <textField/>
         <textField/>
@@ -125,8 +125,8 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="7" name="MLH1_M4_female_glm" type="6" refreshedVersion="5" background="1" saveData="1">
-    <textPr codePage="437" sourceFile="C:\Users\April\Documents\MLH1repo\MLH1_M4_female_glm.csv" comma="1">
+  <connection id="7" name="MLH1_M4_male_glm" type="6" refreshedVersion="5" background="1" saveData="1">
+    <textPr codePage="437" sourceFile="C:\Users\April\Documents\MLH1repo\MLH1_M4_male_glm.csv" tab="0" comma="1">
       <textFields count="5">
         <textField/>
         <textField/>
@@ -136,8 +136,8 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="8" name="MLH1_M4_male_glm" type="6" refreshedVersion="5" background="1" saveData="1">
-    <textPr codePage="437" sourceFile="C:\Users\April\Documents\MLH1repo\MLH1_M4_male_glm.csv" tab="0" comma="1">
+  <connection id="8" name="MLH1_M5_female_glm" type="6" refreshedVersion="5" background="1" saveData="1">
+    <textPr codePage="437" sourceFile="C:\Users\April\Documents\MLH1repo\MLH1_M5_female_glm.csv" comma="1">
       <textFields count="5">
         <textField/>
         <textField/>
@@ -147,8 +147,8 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="9" name="MLH1_M5_female_glm" type="6" refreshedVersion="5" background="1" saveData="1">
-    <textPr codePage="437" sourceFile="C:\Users\April\Documents\MLH1repo\MLH1_M5_female_glm.csv" comma="1">
+  <connection id="9" name="MLH1_M5_male_glm" type="6" refreshedVersion="5" background="1" saveData="1">
+    <textPr codePage="437" sourceFile="C:\Users\April\Documents\MLH1repo\MLH1_M5_male_glm.csv" comma="1">
       <textFields count="5">
         <textField/>
         <textField/>
@@ -158,8 +158,8 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="10" name="MLH1_M5_male_glm" type="6" refreshedVersion="5" background="1" saveData="1">
-    <textPr codePage="437" sourceFile="C:\Users\April\Documents\MLH1repo\MLH1_M5_male_glm.csv" comma="1">
+  <connection id="10" name="Nrm1CO_Pos_Q1_M1" type="6" refreshedVersion="5" background="1" saveData="1">
+    <textPr codePage="437" sourceFile="C:\Users\April\Documents\MLH1repo\Nrm1CO_Pos_Q1_M1.csv" comma="1">
       <textFields count="5">
         <textField/>
         <textField/>
@@ -169,8 +169,8 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="11" name="Nrm1CO_Pos_Q1_M1" type="6" refreshedVersion="5" background="1" saveData="1">
-    <textPr codePage="437" sourceFile="C:\Users\April\Documents\MLH1repo\Nrm1CO_Pos_Q1_M1.csv" comma="1">
+  <connection id="11" name="Nrm1CO_Pos_Q1_M2" type="6" refreshedVersion="5" background="1" saveData="1">
+    <textPr codePage="437" sourceFile="C:\Users\April\Documents\MLH1repo\Nrm1CO_Pos_Q1_M2.csv" comma="1">
       <textFields count="5">
         <textField/>
         <textField/>
@@ -180,8 +180,8 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="12" name="Nrm1CO_Pos_Q1_M2" type="6" refreshedVersion="5" background="1" saveData="1">
-    <textPr codePage="437" sourceFile="C:\Users\April\Documents\MLH1repo\Nrm1CO_Pos_Q1_M2.csv" comma="1">
+  <connection id="12" name="Nrm1CO_Pos_Q1_M3" type="6" refreshedVersion="5" background="1" saveData="1">
+    <textPr codePage="437" sourceFile="C:\Users\April\Documents\MLH1repo\Nrm1CO_Pos_Q1_M3.csv" comma="1">
       <textFields count="5">
         <textField/>
         <textField/>
@@ -191,8 +191,8 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="13" name="Nrm1CO_Pos_Q1_M3" type="6" refreshedVersion="5" background="1" saveData="1">
-    <textPr codePage="437" sourceFile="C:\Users\April\Documents\MLH1repo\Nrm1CO_Pos_Q1_M3.csv" comma="1">
+  <connection id="13" name="PER.IFD_Q1_M2" type="6" refreshedVersion="5" background="1" saveData="1">
+    <textPr codePage="437" sourceFile="C:\Users\April\Documents\MLH1repo\PER.IFD_Q1_M2.csv" comma="1">
       <textFields count="5">
         <textField/>
         <textField/>
@@ -202,8 +202,8 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="14" name="PER.IFD_Q1_M2" type="6" refreshedVersion="5" background="1" saveData="1">
-    <textPr codePage="437" sourceFile="C:\Users\April\Documents\MLH1repo\PER.IFD_Q1_M2.csv" comma="1">
+  <connection id="14" name="PER.IFD_Q1_M3" type="6" refreshedVersion="5" background="1" saveData="1">
+    <textPr codePage="437" sourceFile="C:\Users\April\Documents\MLH1repo\PER.IFD_Q1_M3.csv" comma="1">
       <textFields count="5">
         <textField/>
         <textField/>
@@ -213,8 +213,8 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="15" name="PER.IFD_Q1_M3" type="6" refreshedVersion="5" background="1" saveData="1">
-    <textPr codePage="437" sourceFile="C:\Users\April\Documents\MLH1repo\PER.IFD_Q1_M3.csv" comma="1">
+  <connection id="15" name="ShortSC_Q1_M1" type="6" refreshedVersion="5" background="1" saveData="1">
+    <textPr codePage="437" sourceFile="C:\Users\April\Documents\MLH1repo\ShortSC_Q1_M1.csv" tab="0" comma="1">
       <textFields count="5">
         <textField/>
         <textField/>
@@ -224,8 +224,8 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="16" name="ShortSC_Q1_M1" type="6" refreshedVersion="5" background="1" saveData="1">
-    <textPr codePage="437" sourceFile="C:\Users\April\Documents\MLH1repo\ShortSC_Q1_M1.csv" tab="0" comma="1">
+  <connection id="16" name="ShortSC_Q1_M11" type="6" refreshedVersion="5" background="1" saveData="1">
+    <textPr codePage="437" sourceFile="C:\Users\April\Documents\MLH1repo\ShortSC_Q1_M1.csv" comma="1">
       <textFields count="5">
         <textField/>
         <textField/>
@@ -235,8 +235,8 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="17" name="ShortSC_Q1_M11" type="6" refreshedVersion="5" background="1" saveData="1">
-    <textPr codePage="437" sourceFile="C:\Users\April\Documents\MLH1repo\ShortSC_Q1_M1.csv" comma="1">
+  <connection id="17" name="ShortSC_Q1_M2" type="6" refreshedVersion="5" background="1" saveData="1">
+    <textPr codePage="437" sourceFile="C:\Users\April\Documents\MLH1repo\ShortSC_Q1_M2.csv" comma="1">
       <textFields count="5">
         <textField/>
         <textField/>
@@ -246,8 +246,8 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="18" name="ShortSC_Q1_M2" type="6" refreshedVersion="5" background="1" saveData="1">
-    <textPr codePage="437" sourceFile="C:\Users\April\Documents\MLH1repo\ShortSC_Q1_M2.csv" comma="1">
+  <connection id="18" name="ShortSC_Q1_M3" type="6" refreshedVersion="5" background="1" saveData="1">
+    <textPr codePage="437" sourceFile="C:\Users\April\Documents\MLH1repo\ShortSC_Q1_M3.csv" comma="1">
       <textFields count="5">
         <textField/>
         <textField/>
@@ -257,7 +257,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="19" name="ShortSC_Q1_M3" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="19" name="ShortSC_Q1_M31" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="437" sourceFile="C:\Users\April\Documents\MLH1repo\ShortSC_Q1_M3.csv" comma="1">
       <textFields count="5">
         <textField/>
@@ -268,18 +268,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="20" name="ShortSC_Q1_M31" type="6" refreshedVersion="5" background="1" saveData="1">
-    <textPr codePage="437" sourceFile="C:\Users\April\Documents\MLH1repo\ShortSC_Q1_M3.csv" comma="1">
-      <textFields count="5">
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-      </textFields>
-    </textPr>
-  </connection>
-  <connection id="21" name="TotalSC_Q1_M2" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="20" name="TotalSC_Q1_M2" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="437" sourceFile="C:\Users\April\Documents\MLH1repo\TotalSC_Q1_M2.csv" comma="1">
       <textFields count="5">
         <textField/>
@@ -294,7 +283,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="76">
   <si>
     <t>Estimate</t>
   </si>
@@ -510,6 +499,18 @@
   </si>
   <si>
     <t xml:space="preserve"> Residual             1.89  </t>
+  </si>
+  <si>
+    <t>Subspecies</t>
+  </si>
+  <si>
+    <t>Sex</t>
+  </si>
+  <si>
+    <t>Subspecies*Sex</t>
+  </si>
+  <si>
+    <t>strain(random)</t>
   </si>
 </sst>
 </file>
@@ -612,7 +613,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -644,9 +645,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -669,83 +667,79 @@
 </file>
 
 <file path=xl/queryTables/queryTable10.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ShortSC_Q1_M3" connectionId="19" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable11.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ShortSC_Q1_M1" connectionId="16" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable11.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ShortSC_Q1_M3" connectionId="20" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
 <file path=xl/queryTables/queryTable12.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ShortSC_Q1_M1" connectionId="17" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ShortSC_Q1_M2" connectionId="17" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable13.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ShortSC_Q1_M2" connectionId="18" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Nrm1CO_Pos_Q1_M2" connectionId="11" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable14.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Nrm1CO_Pos_Q1_M1" connectionId="11" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Nrm1CO_Pos_Q1_M3" connectionId="12" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable15.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Nrm1CO_Pos_Q1_M2" connectionId="12" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Nrm1CO_Pos_Q1_M1" connectionId="10" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable16.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Nrm1CO_Pos_Q1_M3" connectionId="13" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ABS.IFD_Q1_M1" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable17.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PER.IFD_Q1_M3" connectionId="15" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ABS.IFD_Q1_M2" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable18.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ABS.IFD_Q1_M1" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PER.IFD_Q1_M2" connectionId="13" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable19.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ABS.IFD_Q1_M2" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ABS.IFD_Q1_M3" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MLH1_M1_glm" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MLH1_M2_glm" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable20.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PER.IFD_Q1_M2" connectionId="14" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable21.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ABS.IFD_Q1_M3" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PER.IFD_Q1_M3" connectionId="14" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MLH1_M2_glm" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MLH1_M5_female_glm" connectionId="8" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MLH1_M5_female_glm" connectionId="9" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MLH1_M4_female_glm" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MLH1_M4_female_glm" connectionId="7" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MLH1_M4_male_glm" connectionId="7" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MLH1_M4_male_glm" connectionId="8" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MLH1_M5_male_glm" connectionId="9" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MLH1_M5_male_glm" connectionId="10" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ShortSC_Q1_M1" connectionId="15" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TotalSC_Q1_M2" connectionId="21" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TotalSC_Q1_M2" connectionId="20" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ShortSC_Q1_M3" connectionId="19" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ShortSC_Q1_M3" connectionId="18" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2199,209 +2193,162 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M22"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="I1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="J1" t="s">
-        <v>47</v>
-      </c>
-      <c r="M1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>28</v>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>64</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="F2" s="8"/>
-      <c r="G2" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="J2">
+        <v>72</v>
+      </c>
+      <c r="C2">
         <v>9.6925034659947054E-4</v>
       </c>
-      <c r="L2" t="s">
+      <c r="F2" t="s">
         <v>65</v>
       </c>
-      <c r="M2">
+      <c r="G2">
         <v>26.356000000000002</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B3">
-        <v>9.6925034659947054E-4</v>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="13"/>
+      <c r="B3" s="8" t="s">
+        <v>73</v>
       </c>
       <c r="C3">
         <v>3.6415960512153727E-6</v>
       </c>
-      <c r="D3">
+      <c r="F3" t="s">
+        <v>66</v>
+      </c>
+      <c r="G3">
+        <v>-0.755</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="13"/>
+      <c r="B4" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C4">
         <v>1.8013460998954285E-4</v>
       </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="G3" s="13"/>
-      <c r="H3" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="J3">
-        <v>3.6415960512153727E-6</v>
-      </c>
-      <c r="L3" t="s">
-        <v>66</v>
-      </c>
-      <c r="M3">
-        <v>-0.755</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>63</v>
-      </c>
-      <c r="G4" s="13"/>
-      <c r="H4" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="J4">
-        <v>1.8013460998954285E-4</v>
-      </c>
-      <c r="L4" t="s">
+      <c r="F4" t="s">
         <v>6</v>
       </c>
-      <c r="M4">
+      <c r="G4">
         <v>-0.48199999999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="G5" s="14"/>
-      <c r="H5" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
-      <c r="L5" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="14"/>
+      <c r="B5" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C5">
+        <f>1/10000</f>
+        <v>1E-4</v>
+      </c>
+      <c r="F5" t="s">
         <v>67</v>
       </c>
-      <c r="M5">
+      <c r="G5">
         <v>-2.649</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="L6" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F6" t="s">
         <v>68</v>
       </c>
-      <c r="M6">
+      <c r="G6">
         <v>2.9529999999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="L7" t="s">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F7" t="s">
         <v>69</v>
       </c>
-      <c r="M7">
+      <c r="G7">
         <v>3.2010000000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F9" s="4" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F10" s="4" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F11" s="4" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F12" s="5" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="F14" s="15"/>
-      <c r="G14" s="8"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="8"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="8"/>
-    </row>
-    <row r="17" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E17" s="15"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="8"/>
-    </row>
-    <row r="19" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="F19" s="15"/>
-      <c r="G19" s="8"/>
-    </row>
-    <row r="20" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E20" s="15"/>
-      <c r="F20" s="15"/>
-      <c r="G20" s="8"/>
-    </row>
-    <row r="21" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="8"/>
-    </row>
-    <row r="22" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E22" s="15"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="8"/>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F13" s="5"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="8"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="8"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="8"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="8"/>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" s="8"/>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" s="8"/>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B21" s="8"/>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B22" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="G2:G5"/>
+    <mergeCell ref="A2:A5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>